<commit_message>
menyimpan perubahan di file excel
</commit_message>
<xml_diff>
--- a/server/assets/REKAP.xlsx
+++ b/server/assets/REKAP.xlsx
@@ -1,43 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a785782fdef4b5cc/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{F8444799-5609-4627-BC5D-BBE8DDB816FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F332253-6D40-4EEE-987F-2E272485B97B}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{3B661740-81DB-4A45-A5CC-168BE1217C08}"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="38235" windowHeight="20820"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="rekap" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
+    <t>9999 9999 99</t>
+  </si>
+  <si>
+    <t>BULAN MARET 2024</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
@@ -69,59 +53,52 @@
   </si>
   <si>
     <t>NIP. 19800830 200212 2 009</t>
-  </si>
-  <si>
-    <t>JADWAL DISTRIBUSI OBAT KE PUSKESMAS</t>
-  </si>
-  <si>
-    <t>BULAN MARET 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <color theme="1"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <sz val="14"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <family val="2"/>
       <sz val="12"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
+      <family val="2"/>
       <sz val="12"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <u/>
+      <family val="2"/>
       <sz val="12"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,9 +121,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -159,7 +134,9 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -219,55 +196,58 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="1" xr:uid="{AD9311F4-8499-4F5C-8746-8AF3F53E44A7}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -598,78 +578,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E54FF01C-D7D9-47B6-B17C-9EB8FD25BF1E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
     <col min="6" max="6" width="66.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="2" ht="18.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" ht="31.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="4" t="s">
-        <v>6</v>
+      <c r="E7" s="6"/>
+      <c r="F7" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -678,7 +659,7 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
@@ -686,7 +667,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="6"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
@@ -694,7 +675,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
@@ -702,8 +683,8 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="5" t="s">
-        <v>6</v>
+      <c r="F11" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -712,7 +693,7 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
@@ -720,7 +701,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
@@ -728,7 +709,7 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -736,8 +717,8 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="5" t="s">
-        <v>6</v>
+      <c r="F15" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -746,7 +727,7 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
@@ -754,7 +735,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
@@ -762,7 +743,7 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
@@ -770,8 +751,8 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="5" t="s">
-        <v>6</v>
+      <c r="F19" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -780,7 +761,7 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="5"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
@@ -788,7 +769,7 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -796,7 +777,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
@@ -804,8 +785,8 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="5" t="s">
-        <v>6</v>
+      <c r="F23" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -814,7 +795,7 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="5"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
@@ -822,7 +803,7 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
@@ -830,7 +811,7 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
@@ -838,8 +819,8 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="5" t="s">
-        <v>6</v>
+      <c r="F27" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -848,7 +829,7 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="5"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
@@ -856,7 +837,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
@@ -864,7 +845,7 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
@@ -872,8 +853,8 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="5" t="s">
-        <v>6</v>
+      <c r="F31" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -882,7 +863,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="5"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
@@ -890,7 +871,7 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
@@ -898,7 +879,7 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
@@ -906,8 +887,8 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="F35" s="5" t="s">
-        <v>6</v>
+      <c r="F35" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,7 +897,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
-      <c r="F36" s="5"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
@@ -924,7 +905,7 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
@@ -932,7 +913,7 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
@@ -940,8 +921,8 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
-      <c r="F39" s="5" t="s">
-        <v>6</v>
+      <c r="F39" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -950,7 +931,7 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
-      <c r="F40" s="5"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
@@ -958,7 +939,7 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
@@ -966,7 +947,7 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
@@ -974,8 +955,8 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
-      <c r="F43" s="5" t="s">
-        <v>6</v>
+      <c r="F43" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -984,7 +965,7 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
-      <c r="F44" s="5"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
@@ -992,7 +973,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="F45" s="11"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
@@ -1000,7 +981,7 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
+      <c r="F46" s="11"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
@@ -1008,8 +989,8 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
-      <c r="F47" s="5" t="s">
-        <v>6</v>
+      <c r="F47" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1018,87 +999,87 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F49" s="11"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F57" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G57" s="11"/>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F58" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G58" s="11"/>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F62" s="13" t="s">
+      <c r="F50" s="11"/>
+    </row>
+    <row r="51" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="13"/>
+    </row>
+    <row r="57" ht="15.75" customHeight="1" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F57" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G62" s="13"/>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F63" s="14" t="s">
+      <c r="G57" s="14"/>
+    </row>
+    <row r="58" ht="15.75" customHeight="1" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F58" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G63" s="14"/>
+      <c r="G58" s="14"/>
+    </row>
+    <row r="59" ht="15.75" customHeight="1" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+    </row>
+    <row r="60" ht="15.75" customHeight="1" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+    </row>
+    <row r="61" ht="15.75" customHeight="1" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+    </row>
+    <row r="62" ht="15.75" customHeight="1" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F62" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G62" s="16"/>
+    </row>
+    <row r="63" ht="15.75" customHeight="1" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F63" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F23:F24"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="F35:F36"/>
     <mergeCell ref="F39:F40"/>
     <mergeCell ref="F43:F44"/>
     <mergeCell ref="F47:F48"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>